<commit_message>
paper is 3.5 pages right now
</commit_message>
<xml_diff>
--- a/10FoldXVal/Graph.xlsx
+++ b/10FoldXVal/Graph.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="32">
   <si>
     <t>100% Confidence</t>
   </si>
@@ -73,6 +73,45 @@
   </si>
   <si>
     <t>95% Confidence</t>
+  </si>
+  <si>
+    <t>Rules created</t>
+  </si>
+  <si>
+    <t>Complement1</t>
+  </si>
+  <si>
+    <t>Complement2</t>
+  </si>
+  <si>
+    <t>Complement3</t>
+  </si>
+  <si>
+    <t>Complement4</t>
+  </si>
+  <si>
+    <t>Complement5</t>
+  </si>
+  <si>
+    <t>Complement6</t>
+  </si>
+  <si>
+    <t>Complement7</t>
+  </si>
+  <si>
+    <t>Complement8</t>
+  </si>
+  <si>
+    <t>Complement9</t>
+  </si>
+  <si>
+    <t>Complement10</t>
+  </si>
+  <si>
+    <t>Number of rules</t>
+  </si>
+  <si>
+    <t>In percentage form</t>
   </si>
 </sst>
 </file>
@@ -108,9 +147,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -171,9 +211,9 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="0.13714892802697692"/>
-          <c:y val="0.16714129483814524"/>
-          <c:w val="0.60953583504764608"/>
-          <c:h val="0.63527173510090895"/>
+          <c:y val="0.22363835876447646"/>
+          <c:w val="0.72244874796055891"/>
+          <c:h val="0.61643934338716133"/>
         </c:manualLayout>
       </c:layout>
       <c:barChart>
@@ -344,13 +384,116 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:gapWidth val="150"/>
+        <c:gapWidth val="99"/>
         <c:overlap val="100"/>
-        <c:axId val="168257408"/>
-        <c:axId val="168259584"/>
+        <c:axId val="44020864"/>
+        <c:axId val="44023168"/>
+      </c:barChart>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$C$21</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Number of rules</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:pattFill prst="ltUpDiag">
+              <a:fgClr>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:fgClr>
+              <a:bgClr>
+                <a:schemeClr val="bg1"/>
+              </a:bgClr>
+            </a:pattFill>
+            <a:ln w="22225">
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:pattFill prst="ltUpDiag">
+                <a:fgClr>
+                  <a:schemeClr val="accent1">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:fgClr>
+                <a:bgClr>
+                  <a:schemeClr val="bg1"/>
+                </a:bgClr>
+              </a:pattFill>
+              <a:ln w="22225">
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$D$17:$F$17</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.95</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$21:$F$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>2837.2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2134.3000000000002</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1484.6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="500"/>
+        <c:axId val="48734592"/>
+        <c:axId val="48588672"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="168257408"/>
+        <c:axId val="44020864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -397,7 +540,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="168259584"/>
+        <c:crossAx val="44023168"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -405,7 +548,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="168259584"/>
+        <c:axId val="44023168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -432,8 +575,8 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="9.2791374051216565E-3"/>
-              <c:y val="0.1483087919094859"/>
+              <c:x val="1.4083942209926462E-2"/>
+              <c:y val="0.20857244539347836"/>
             </c:manualLayout>
           </c:layout>
           <c:overlay val="0"/>
@@ -442,21 +585,73 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="168257408"/>
+        <c:crossAx val="44020864"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
+      <c:valAx>
+        <c:axId val="48588672"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="r"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1400"/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1400"/>
+                  <a:t>Number of association rules</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="48734592"/>
+        <c:crosses val="max"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:catAx>
+        <c:axId val="48734592"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="0%" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="48588672"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
     </c:plotArea>
     <c:legend>
-      <c:legendPos val="r"/>
+      <c:legendPos val="t"/>
       <c:layout>
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.75327611075642575"/>
-          <c:y val="0.39169358067529697"/>
-          <c:w val="0.24523799389941123"/>
-          <c:h val="0.23167845544730636"/>
+          <c:x val="5.7207254498593083E-2"/>
+          <c:y val="0.11299435028248588"/>
+          <c:w val="0.8999999054172283"/>
+          <c:h val="7.7226151815768779E-2"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -489,14 +684,14 @@
     <xdr:from>
       <xdr:col>11</xdr:col>
       <xdr:colOff>85725</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
       <xdr:colOff>495300</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -805,13 +1000,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T20"/>
+  <dimension ref="A1:T40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="X25" sqref="X25"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="6" width="9.5703125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -1320,6 +1518,244 @@
       </c>
       <c r="F20">
         <v>72.8</v>
+      </c>
+    </row>
+    <row r="21" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C21" t="s">
+        <v>30</v>
+      </c>
+      <c r="D21">
+        <v>2837.2</v>
+      </c>
+      <c r="E21">
+        <v>2134.3000000000002</v>
+      </c>
+      <c r="F21">
+        <v>1484.6</v>
+      </c>
+    </row>
+    <row r="23" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C23" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="24" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C24" t="s">
+        <v>15</v>
+      </c>
+      <c r="D24" s="2">
+        <f>D18*100/117.7</f>
+        <v>94.137638062871702</v>
+      </c>
+      <c r="E24" s="2">
+        <f t="shared" ref="E24:F24" si="3">E18*100/117.7</f>
+        <v>93.797790994052676</v>
+      </c>
+      <c r="F24" s="2">
+        <f t="shared" si="3"/>
+        <v>35.853865760407814</v>
+      </c>
+    </row>
+    <row r="25" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C25" t="s">
+        <v>17</v>
+      </c>
+      <c r="D25" s="2">
+        <f>D19*100/117.7</f>
+        <v>1.8691588785046731</v>
+      </c>
+      <c r="E25" s="2">
+        <f t="shared" ref="E25:F25" si="4">E19*100/117.7</f>
+        <v>2.0390824129141887</v>
+      </c>
+      <c r="F25" s="2">
+        <f t="shared" si="4"/>
+        <v>2.293967714528462</v>
+      </c>
+    </row>
+    <row r="26" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C26" t="s">
+        <v>30</v>
+      </c>
+      <c r="D26" s="2">
+        <f>D20*100/117.7</f>
+        <v>3.9932030586236191</v>
+      </c>
+      <c r="E26" s="2">
+        <f t="shared" ref="E26:F26" si="5">E20*100/117.7</f>
+        <v>4.1631265930331356</v>
+      </c>
+      <c r="F26" s="2">
+        <f t="shared" si="5"/>
+        <v>61.852166525063723</v>
+      </c>
+    </row>
+    <row r="29" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C29" t="s">
+        <v>19</v>
+      </c>
+      <c r="D29" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="E29" s="1">
+        <v>0.95</v>
+      </c>
+      <c r="F29" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C30" t="s">
+        <v>20</v>
+      </c>
+      <c r="D30">
+        <v>2858</v>
+      </c>
+      <c r="E30">
+        <v>1978</v>
+      </c>
+      <c r="F30">
+        <v>1346</v>
+      </c>
+    </row>
+    <row r="31" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C31" t="s">
+        <v>21</v>
+      </c>
+      <c r="D31">
+        <v>1938</v>
+      </c>
+      <c r="E31">
+        <v>2189</v>
+      </c>
+      <c r="F31">
+        <v>1464</v>
+      </c>
+    </row>
+    <row r="32" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C32" t="s">
+        <v>22</v>
+      </c>
+      <c r="D32">
+        <v>3000</v>
+      </c>
+      <c r="E32">
+        <v>2411</v>
+      </c>
+      <c r="F32">
+        <v>1699</v>
+      </c>
+    </row>
+    <row r="33" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C33" t="s">
+        <v>23</v>
+      </c>
+      <c r="D33">
+        <v>2981</v>
+      </c>
+      <c r="E33">
+        <v>2109</v>
+      </c>
+      <c r="F33">
+        <v>1416</v>
+      </c>
+    </row>
+    <row r="34" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C34" t="s">
+        <v>24</v>
+      </c>
+      <c r="D34">
+        <v>2718</v>
+      </c>
+      <c r="E34">
+        <v>2062</v>
+      </c>
+      <c r="F34">
+        <v>1396</v>
+      </c>
+    </row>
+    <row r="35" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C35" t="s">
+        <v>25</v>
+      </c>
+      <c r="D35">
+        <v>2874</v>
+      </c>
+      <c r="E35">
+        <v>2063</v>
+      </c>
+      <c r="F35">
+        <v>1491</v>
+      </c>
+    </row>
+    <row r="36" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C36" t="s">
+        <v>26</v>
+      </c>
+      <c r="D36">
+        <v>2885</v>
+      </c>
+      <c r="E36">
+        <v>2096</v>
+      </c>
+      <c r="F36">
+        <v>1589</v>
+      </c>
+    </row>
+    <row r="37" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C37" t="s">
+        <v>27</v>
+      </c>
+      <c r="D37">
+        <v>3206</v>
+      </c>
+      <c r="E37">
+        <v>2170</v>
+      </c>
+      <c r="F37">
+        <v>1550</v>
+      </c>
+    </row>
+    <row r="38" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C38" t="s">
+        <v>28</v>
+      </c>
+      <c r="D38">
+        <v>2899</v>
+      </c>
+      <c r="E38">
+        <v>2170</v>
+      </c>
+      <c r="F38">
+        <v>1478</v>
+      </c>
+    </row>
+    <row r="39" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C39" t="s">
+        <v>29</v>
+      </c>
+      <c r="D39">
+        <v>3013</v>
+      </c>
+      <c r="E39">
+        <v>2095</v>
+      </c>
+      <c r="F39">
+        <v>1417</v>
+      </c>
+    </row>
+    <row r="40" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="D40">
+        <f>AVERAGE(D30:D39)</f>
+        <v>2837.2</v>
+      </c>
+      <c r="E40">
+        <f t="shared" ref="E40:F40" si="6">AVERAGE(E30:E39)</f>
+        <v>2134.3000000000002</v>
+      </c>
+      <c r="F40">
+        <f t="shared" si="6"/>
+        <v>1484.6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
modified the graphs file
</commit_message>
<xml_diff>
--- a/10FoldXVal/Graph.xlsx
+++ b/10FoldXVal/Graph.xlsx
@@ -1003,7 +1003,7 @@
   <dimension ref="A1:T40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1541,7 +1541,7 @@
     </row>
     <row r="24" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C24" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D24" s="2">
         <f>D18*100/117.7</f>
@@ -1558,7 +1558,7 @@
     </row>
     <row r="25" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C25" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D25" s="2">
         <f>D19*100/117.7</f>
@@ -1575,7 +1575,7 @@
     </row>
     <row r="26" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C26" t="s">
-        <v>30</v>
+        <v>17</v>
       </c>
       <c r="D26" s="2">
         <f>D20*100/117.7</f>

</xml_diff>